<commit_message>
fix: formatos de ejemplos xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/templates_files/Datos de aspirantes.xlsx
+++ b/src/main/resources/templates_files/Datos de aspirantes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sainos\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9FF8DB-409F-4A91-9A18-21B788881612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8D55E6-08A4-4247-B9F2-9CB58AEB0C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>Número Ficha</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>GRBH010228HOCNRLA7</t>
+  </si>
+  <si>
+    <t>13/30/2025</t>
   </si>
 </sst>
 </file>
@@ -210,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -228,6 +231,9 @@
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -570,7 +576,9 @@
       <c r="F2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -592,7 +600,9 @@
       <c r="F3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -614,7 +624,9 @@
       <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="7"/>
+      <c r="G4" s="7">
+        <v>45943</v>
+      </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -680,7 +692,9 @@
       <c r="F7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="7">
+        <v>45943.395833333336</v>
+      </c>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -724,7 +738,9 @@
       <c r="F9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="7"/>
+      <c r="G9" s="7">
+        <v>45943</v>
+      </c>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>